<commit_message>
ss add , retry and multi browser
</commit_message>
<xml_diff>
--- a/E-Commerce/src/test/ resources/RegistrationData.xlsx
+++ b/E-Commerce/src/test/ resources/RegistrationData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29103"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CFE6C1F-22CA-4860-AD71-2DFC2AEB59DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{20AEA55D-5F48-4A00-BA89-AA92340D88CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
   <si>
     <t>Gender</t>
   </si>
@@ -60,10 +60,31 @@
     <t>Tawade</t>
   </si>
   <si>
-    <t>Chaitanyatawade@gmail.com</t>
+    <t>Chaitanyatawade1@gmail.com</t>
   </si>
   <si>
     <t>Abc@123</t>
+  </si>
+  <si>
+    <t>Om</t>
+  </si>
+  <si>
+    <t>Chaitanyatawade2@gmail.com</t>
+  </si>
+  <si>
+    <t>Nitesh</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Jyoti</t>
+  </si>
+  <si>
+    <t>Deepak</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -123,10 +144,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -462,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -518,9 +540,114 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{DE49DAFC-0B18-4484-B3BF-578F9B25FDF9}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{F261F613-EA0D-446F-B354-BF5151BA8C11}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{AC3CE38D-1B7F-43D2-B1C1-5130E035A235}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{3A35B61F-9874-4522-8581-511BA58E3F0A}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{B59E20DF-2FFB-42D2-9245-C197FAF4729C}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{A9C8DDD3-FFA7-4C3D-98AC-E1CAB32742EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>